<commit_message>
3.3 files (including some temp US placeholders)
</commit_message>
<xml_diff>
--- a/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
+++ b/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaxolt/Google Drive/2021/D.Development/TARGET_eps-us-3.2.1/InputData/elec/BRPSPTY/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Mexico\InputData\elec\BRPSPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF05D635-8D6C-CB42-8F76-0F1A1A34713A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F640757C-CD9B-4CDE-A6C9-0152E3F9E6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30780" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8535" yWindow="1185" windowWidth="19740" windowHeight="11910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>BRPSPTY BAU Renewable Portfolio Std Percentage This Year</t>
   </si>
@@ -92,6 +92,258 @@
   </si>
   <si>
     <t>As current legislative action seems to ignore RPS targets, none will be modeled in BAU.</t>
+  </si>
+  <si>
+    <t>Year2020</t>
+  </si>
+  <si>
+    <t>Year2021</t>
+  </si>
+  <si>
+    <t>Year2022</t>
+  </si>
+  <si>
+    <t>Year2023</t>
+  </si>
+  <si>
+    <t>Year2024</t>
+  </si>
+  <si>
+    <t>Year2025</t>
+  </si>
+  <si>
+    <t>Year2026</t>
+  </si>
+  <si>
+    <t>Year2027</t>
+  </si>
+  <si>
+    <t>Year2028</t>
+  </si>
+  <si>
+    <t>Year2029</t>
+  </si>
+  <si>
+    <t>Year2030</t>
+  </si>
+  <si>
+    <t>Year2031</t>
+  </si>
+  <si>
+    <t>Year2032</t>
+  </si>
+  <si>
+    <t>Year2033</t>
+  </si>
+  <si>
+    <t>Year2034</t>
+  </si>
+  <si>
+    <t>Year2035</t>
+  </si>
+  <si>
+    <t>Year2036</t>
+  </si>
+  <si>
+    <t>Year2037</t>
+  </si>
+  <si>
+    <t>Year2038</t>
+  </si>
+  <si>
+    <t>Year2039</t>
+  </si>
+  <si>
+    <t>Year2040</t>
+  </si>
+  <si>
+    <t>Year2041</t>
+  </si>
+  <si>
+    <t>Year2042</t>
+  </si>
+  <si>
+    <t>Year2043</t>
+  </si>
+  <si>
+    <t>Year2044</t>
+  </si>
+  <si>
+    <t>Year2045</t>
+  </si>
+  <si>
+    <t>Year2046</t>
+  </si>
+  <si>
+    <t>Year2047</t>
+  </si>
+  <si>
+    <t>Year2048</t>
+  </si>
+  <si>
+    <t>Year2049</t>
+  </si>
+  <si>
+    <t>Year2050</t>
+  </si>
+  <si>
+    <t>Year2051</t>
+  </si>
+  <si>
+    <t>Year2052</t>
+  </si>
+  <si>
+    <t>Year2053</t>
+  </si>
+  <si>
+    <t>Year2054</t>
+  </si>
+  <si>
+    <t>Year2055</t>
+  </si>
+  <si>
+    <t>Year2056</t>
+  </si>
+  <si>
+    <t>Year2057</t>
+  </si>
+  <si>
+    <t>Year2058</t>
+  </si>
+  <si>
+    <t>Year2059</t>
+  </si>
+  <si>
+    <t>Year2060</t>
+  </si>
+  <si>
+    <t>Year2061</t>
+  </si>
+  <si>
+    <t>Year2062</t>
+  </si>
+  <si>
+    <t>Year2063</t>
+  </si>
+  <si>
+    <t>Year2064</t>
+  </si>
+  <si>
+    <t>Year2065</t>
+  </si>
+  <si>
+    <t>Year2066</t>
+  </si>
+  <si>
+    <t>Year2067</t>
+  </si>
+  <si>
+    <t>Year2068</t>
+  </si>
+  <si>
+    <t>Year2069</t>
+  </si>
+  <si>
+    <t>Year2070</t>
+  </si>
+  <si>
+    <t>Year2071</t>
+  </si>
+  <si>
+    <t>Year2072</t>
+  </si>
+  <si>
+    <t>Year2073</t>
+  </si>
+  <si>
+    <t>Year2074</t>
+  </si>
+  <si>
+    <t>Year2075</t>
+  </si>
+  <si>
+    <t>Year2076</t>
+  </si>
+  <si>
+    <t>Year2077</t>
+  </si>
+  <si>
+    <t>Year2078</t>
+  </si>
+  <si>
+    <t>Year2079</t>
+  </si>
+  <si>
+    <t>Year2080</t>
+  </si>
+  <si>
+    <t>Year2081</t>
+  </si>
+  <si>
+    <t>Year2082</t>
+  </si>
+  <si>
+    <t>Year2083</t>
+  </si>
+  <si>
+    <t>Year2084</t>
+  </si>
+  <si>
+    <t>Year2085</t>
+  </si>
+  <si>
+    <t>Year2086</t>
+  </si>
+  <si>
+    <t>Year2087</t>
+  </si>
+  <si>
+    <t>Year2088</t>
+  </si>
+  <si>
+    <t>Year2089</t>
+  </si>
+  <si>
+    <t>Year2090</t>
+  </si>
+  <si>
+    <t>Year2091</t>
+  </si>
+  <si>
+    <t>Year2092</t>
+  </si>
+  <si>
+    <t>Year2093</t>
+  </si>
+  <si>
+    <t>Year2094</t>
+  </si>
+  <si>
+    <t>Year2095</t>
+  </si>
+  <si>
+    <t>Year2096</t>
+  </si>
+  <si>
+    <t>Year2097</t>
+  </si>
+  <si>
+    <t>Year2098</t>
+  </si>
+  <si>
+    <t>Year2099</t>
+  </si>
+  <si>
+    <t>Year2100</t>
+  </si>
+  <si>
+    <t>Year2019</t>
+  </si>
+  <si>
+    <t>Year2018</t>
+  </si>
+  <si>
+    <t>Year2017</t>
   </si>
 </sst>
 </file>
@@ -99,9 +351,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -657,14 +909,17 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -713,7 +968,7 @@
     <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Parent row" xfId="46" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Table title" xfId="45" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
@@ -1055,22 +1310,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="122.6640625" customWidth="1"/>
+    <col min="2" max="2" width="122.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1078,30 +1333,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1117,123 +1372,275 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:CG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>2017</v>
-      </c>
-      <c r="C1">
-        <v>2018</v>
-      </c>
-      <c r="D1">
-        <v>2019</v>
-      </c>
-      <c r="E1">
-        <v>2020</v>
-      </c>
-      <c r="F1">
-        <v>2021</v>
-      </c>
-      <c r="G1">
-        <v>2022</v>
-      </c>
-      <c r="H1">
-        <v>2023</v>
-      </c>
-      <c r="I1">
-        <v>2024</v>
-      </c>
-      <c r="J1">
-        <v>2025</v>
-      </c>
-      <c r="K1">
-        <v>2026</v>
-      </c>
-      <c r="L1">
-        <v>2027</v>
-      </c>
-      <c r="M1">
-        <v>2028</v>
-      </c>
-      <c r="N1">
-        <v>2029</v>
-      </c>
-      <c r="O1">
-        <v>2030</v>
-      </c>
-      <c r="P1">
-        <v>2031</v>
-      </c>
-      <c r="Q1">
-        <v>2032</v>
-      </c>
-      <c r="R1">
-        <v>2033</v>
-      </c>
-      <c r="S1">
-        <v>2034</v>
-      </c>
-      <c r="T1">
-        <v>2035</v>
-      </c>
-      <c r="U1">
-        <v>2036</v>
-      </c>
-      <c r="V1">
-        <v>2037</v>
-      </c>
-      <c r="W1">
-        <v>2038</v>
-      </c>
-      <c r="X1">
-        <v>2039</v>
-      </c>
-      <c r="Y1">
-        <v>2040</v>
-      </c>
-      <c r="Z1">
-        <v>2041</v>
-      </c>
-      <c r="AA1">
-        <v>2042</v>
-      </c>
-      <c r="AB1">
-        <v>2043</v>
-      </c>
-      <c r="AC1">
-        <v>2044</v>
-      </c>
-      <c r="AD1">
-        <v>2045</v>
-      </c>
-      <c r="AE1">
-        <v>2046</v>
-      </c>
-      <c r="AF1">
-        <v>2047</v>
-      </c>
-      <c r="AG1">
-        <v>2048</v>
-      </c>
-      <c r="AH1">
-        <v>2049</v>
-      </c>
-      <c r="AI1">
-        <v>2050</v>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AW1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AY1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BC1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BG1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BI1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="BJ1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="BL1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="BM1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="BN1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BO1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="BP1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BQ1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="BR1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BS1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="BT1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="BU1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="BV1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BW1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="BX1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="BY1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="BZ1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="CA1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="CB1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="CC1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="CD1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="CE1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="CF1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="CG1" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="32">
+    <row r="2" spans="1:85" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1337,10 +1744,161 @@
         <v>0</v>
       </c>
       <c r="AI2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BK2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BL2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BN2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BO2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BP2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BQ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BR2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BS2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BT2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BU2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BV2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BW2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BX2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BY2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BZ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="CA2" s="4">
+        <v>0</v>
+      </c>
+      <c r="CB2" s="4">
+        <v>0</v>
+      </c>
+      <c r="CC2" s="4">
+        <v>0</v>
+      </c>
+      <c r="CD2" s="4">
+        <v>0</v>
+      </c>
+      <c r="CE2" s="4">
+        <v>0</v>
+      </c>
+      <c r="CF2" s="4">
+        <v>0</v>
+      </c>
+      <c r="CG2" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated RPS with current policy values
</commit_message>
<xml_diff>
--- a/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
+++ b/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Mexico\InputData\elec\BRPSPTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ssy02/Desktop/240925-eps-mx/InputData/elec/BRPSPTY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F640757C-CD9B-4CDE-A6C9-0152E3F9E6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4BA2DE-FA7D-4F4B-96C1-2ACC8B5AA3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8535" yWindow="1185" windowWidth="19740" windowHeight="11910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -88,12 +88,6 @@
     <t>RPS Fraction (dimensionless)</t>
   </si>
   <si>
-    <t xml:space="preserve">In Mexico there is no renewable energy target for BAU, therefore all the values are 0. </t>
-  </si>
-  <si>
-    <t>As current legislative action seems to ignore RPS targets, none will be modeled in BAU.</t>
-  </si>
-  <si>
     <t>Year2020</t>
   </si>
   <si>
@@ -344,6 +338,14 @@
   </si>
   <si>
     <t>Year2017</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy22osti/82580.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexico’s energy transition law established a target for meeting at
+least 35% of its electricity generation from clean energy sources
+by 2024. </t>
   </si>
 </sst>
 </file>
@@ -353,7 +355,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,6 +513,14 @@
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -846,7 +856,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -908,11 +918,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -920,8 +930,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="51"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="52">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
@@ -959,6 +970,7 @@
     <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8"/>
     <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
@@ -988,9 +1000,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1028,9 +1040,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1063,26 +1075,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1115,26 +1110,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1308,62 +1286,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="122.7109375" customWidth="1"/>
+    <col min="2" max="2" width="122.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="48">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="B3" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
+      <c r="B5" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{81E5C5BB-D9CE-3741-AEFA-FBEEF3FF9DED}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1375,526 +1353,526 @@
   <dimension ref="A1:CG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:CG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:85">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AA1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AB1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AC1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AD1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AE1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AF1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AG1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AH1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AI1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AK1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AL1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AM1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AN1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AO1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AP1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AR1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AS1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AT1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AU1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AV1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AW1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AX1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AY1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="BA1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="BB1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BC1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BD1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BE1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BF1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BG1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BH1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BG1" s="5" t="s">
+      <c r="BI1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BH1" s="5" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BI1" s="5" t="s">
+      <c r="BK1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BJ1" s="5" t="s">
+      <c r="BL1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BK1" s="5" t="s">
+      <c r="BM1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BL1" s="5" t="s">
+      <c r="BN1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BM1" s="5" t="s">
+      <c r="BO1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BN1" s="5" t="s">
+      <c r="BP1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BO1" s="5" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BP1" s="5" t="s">
+      <c r="BR1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="BQ1" s="5" t="s">
+      <c r="BS1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BR1" s="5" t="s">
+      <c r="BT1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="BS1" s="5" t="s">
+      <c r="BU1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BT1" s="5" t="s">
+      <c r="BV1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="BU1" s="5" t="s">
+      <c r="BW1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="BV1" s="5" t="s">
+      <c r="BX1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BW1" s="5" t="s">
+      <c r="BY1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BX1" s="5" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BY1" s="5" t="s">
+      <c r="CA1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BZ1" s="5" t="s">
+      <c r="CB1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="CA1" s="5" t="s">
+      <c r="CC1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="CB1" s="5" t="s">
+      <c r="CD1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="CC1" s="5" t="s">
+      <c r="CE1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="CD1" s="5" t="s">
+      <c r="CF1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="CE1" s="5" t="s">
+      <c r="CG1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="CF1" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="CG1" s="5" t="s">
-        <v>90</v>
-      </c>
     </row>
-    <row r="2" spans="1:85" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:85" ht="32">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4">
-        <v>0</v>
-      </c>
-      <c r="O2" s="4">
-        <v>0</v>
-      </c>
-      <c r="P2" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>0</v>
-      </c>
-      <c r="R2" s="4">
-        <v>0</v>
-      </c>
-      <c r="S2" s="4">
-        <v>0</v>
-      </c>
-      <c r="T2" s="4">
-        <v>0</v>
-      </c>
-      <c r="U2" s="4">
-        <v>0</v>
-      </c>
-      <c r="V2" s="4">
-        <v>0</v>
-      </c>
-      <c r="W2" s="4">
-        <v>0</v>
-      </c>
-      <c r="X2" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AT2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AV2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AX2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AY2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BA2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BB2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BC2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BD2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BE2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BF2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BG2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BH2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BI2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BJ2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BK2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BL2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BM2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BN2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BO2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BP2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BQ2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BR2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BS2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BT2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BU2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BV2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BW2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BX2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BY2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BZ2" s="4">
-        <v>0</v>
-      </c>
-      <c r="CA2" s="4">
-        <v>0</v>
-      </c>
-      <c r="CB2" s="4">
-        <v>0</v>
-      </c>
-      <c r="CC2" s="4">
-        <v>0</v>
-      </c>
-      <c r="CD2" s="4">
-        <v>0</v>
-      </c>
-      <c r="CE2" s="4">
-        <v>0</v>
-      </c>
-      <c r="CF2" s="4">
-        <v>0</v>
-      </c>
-      <c r="CG2" s="4">
-        <v>0</v>
+      <c r="B2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="V2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="W2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="X2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AH2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AI2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AJ2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AK2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AL2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AM2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AN2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AO2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AP2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AQ2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AR2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AS2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AT2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AU2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AV2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AW2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AX2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AY2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="AZ2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BA2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BB2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BC2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BD2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BE2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BF2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BG2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BH2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BI2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BJ2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BK2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BL2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BM2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BN2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BO2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BP2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BQ2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BR2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BS2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BT2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BU2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BV2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BW2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BX2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BY2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="BZ2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="CA2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="CB2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="CC2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="CD2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="CE2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="CF2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="CG2" s="3">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>